<commit_message>
Ajout graphiques, resultats enregistres
</commit_message>
<xml_diff>
--- a/Regression/save_test.xlsx
+++ b/Regression/save_test.xlsx
@@ -7,15 +7,138 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sans_norm" sheetId="1" r:id="rId1"/>
-    <sheet name="Normalisees" sheetId="2" r:id="rId2"/>
+    <sheet name="Correlations" sheetId="1" r:id="rId1"/>
+    <sheet name="Resultats non-norm" sheetId="2" r:id="rId2"/>
+    <sheet name="Sans_norm" sheetId="3" r:id="rId3"/>
+    <sheet name="Resultats norm" sheetId="4" r:id="rId4"/>
+    <sheet name="Normalisees" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+  <si>
+    <t>Corr w/ TAUX_OCC</t>
+  </si>
+  <si>
+    <t>SELECT</t>
+  </si>
+  <si>
+    <t>NOM_HOSPITAL</t>
+  </si>
+  <si>
+    <t>NB_PATIENT_CIV_24_H</t>
+  </si>
+  <si>
+    <t>NB_PATIENT_CIV_48_H</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>HUMIDITY</t>
+  </si>
+  <si>
+    <t>PRESSURE</t>
+  </si>
+  <si>
+    <t>VISIBILITY</t>
+  </si>
+  <si>
+    <t>WIND_SPEED</t>
+  </si>
+  <si>
+    <t>WEATHER</t>
+  </si>
+  <si>
+    <t>WEATHER_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>MOIS</t>
+  </si>
+  <si>
+    <t>HEURE</t>
+  </si>
+  <si>
+    <t>JOUR</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Erreur</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP',
+       'PRESSURE'],
+      dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP',
+       'PRESSURE', 'JOUR'],
+      dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_24_H'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP', 'PRESSURE'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP', 'PRESSURE',
+       'JOUR'],
+      dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_48_H'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_48_H', 'TEMP'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_48_H', 'TEMP', 'PRESSURE'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['NB_PATIENT_CIV_48_H', 'TEMP', 'PRESSURE', 'JOUR'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['TEMP'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['TEMP', 'PRESSURE'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['TEMP', 'PRESSURE', 'JOUR'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['PRESSURE'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['PRESSURE', 'JOUR'], dtype='object')</t>
+  </si>
+  <si>
+    <t>Index(['JOUR'], dtype='object')</t>
+  </si>
   <si>
     <t>Sans normalisation</t>
   </si>
@@ -24,12 +147,6 @@
   </si>
   <si>
     <t>err</t>
-  </si>
-  <si>
-    <t>Index(['NOM_HOSPITAL', 'NB_PATIENT_CIV_24_H', 'NB_PATIENT_CIV_48_H', 'TEMP',
-       'HUMIDITY', 'PRESSURE', 'VISIBILITY', 'WIND_SPEED', 'WEATHER',
-       'WEATHER_DESCRIPTION', 'MOIS', 'HEURE', 'JOUR'],
-      dtype='object')</t>
   </si>
   <si>
     <t>Donnees normalisees</t>
@@ -390,31 +507,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>-0.2486644867329692</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="B3">
-        <v>0.7355200350998512</v>
+        <v>0.4287219915821286</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.3007725037600397</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.1021728389844536</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>-0.04470581606881564</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>-0.1315651278980553</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.03434497937673003</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>-0.05776606655836294</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>-0.008565981247831405</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>-0.008006573155245002</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.04946730126650513</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>0.03065278271768995</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>-0.1264366933798786</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -423,6 +670,258 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>0.890911878214939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>0.8005639093276603</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>0.8011292545639336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>0.800181732068912</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>0.7886489863878503</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>0.7784281466173635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>0.8173416703172602</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0.8177116582562038</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>0.8163303653335109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.8039795150245957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>0.793253005575696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>0.9109818745462274</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0.9082925158278977</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>0.9035225976184084</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>0.8941037048251882</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>0.9910689253877067</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>0.9810980719657337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>0.9648837702359091</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>0.9852180438915314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>0.9706723924893805</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>0.9857753595286111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -432,23 +931,309 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3">
+        <v>0.7784281466173635</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <v>0.890911878214939</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>0.8005499722098813</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4">
+        <v>0.8010684741702391</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>0.8001228232208905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>0.7885896312403822</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>0.7783688246686203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>0.8173567510648633</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9">
+        <v>0.8177058084085864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10">
+        <v>0.8163246537516321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11">
+        <v>0.8039812672382984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12">
+        <v>0.7932514428936693</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13">
+        <v>0.9109817419090968</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14">
+        <v>0.9082897613569517</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>0.9035207221039826</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>0.8941002039453898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>0.9910692089358867</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18">
+        <v>0.9810925602819455</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19">
+        <v>0.9648769328900766</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20">
+        <v>0.9852142042829047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21">
+        <v>0.9706671367061587</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>0.9857753595286111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="B3">
-        <v>0.735474081934666</v>
+        <v>0.7783688246686203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>